<commit_message>
excel update + more work done on servo paint
</commit_message>
<xml_diff>
--- a/camera meeting.xlsx
+++ b/camera meeting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriaan\Documents\school\Minor SMR\Eurofins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriaan\Documents\school\Minor SMR\Eurofins\SMR-2-Eurofins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2367C316-EAF0-48B5-8F9C-EB756DADCC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D788FDDA-6ACC-45C9-A04D-A37424CF2951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17504D4C-2CC1-4FF1-A566-434FCFBC1EB6}"/>
   </bookViews>
@@ -35,8 +35,70 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="5">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="5">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>sample 1</t>
   </si>
@@ -47,12 +109,6 @@
     <t>sample 3</t>
   </si>
   <si>
-    <t>pixsel backbone</t>
-  </si>
-  <si>
-    <t>pixsel sample</t>
-  </si>
-  <si>
     <t>irl backbone (mm)</t>
   </si>
   <si>
@@ -72,6 +128,30 @@
   </si>
   <si>
     <t>sample 4-</t>
+  </si>
+  <si>
+    <t>sample 4+-</t>
+  </si>
+  <si>
+    <t>4+ is aan de hoge kant gemeten</t>
+  </si>
+  <si>
+    <t>4- is aan de lage kant gemeten</t>
+  </si>
+  <si>
+    <t>pixsl backbone</t>
+  </si>
+  <si>
+    <t>pixel sample</t>
+  </si>
+  <si>
+    <t>irl = in real life</t>
+  </si>
+  <si>
+    <t>dif = difference</t>
+  </si>
+  <si>
+    <t>Sample height  (mm)</t>
   </si>
 </sst>
 </file>
@@ -93,15 +173,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,12 +201,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -130,6 +247,90 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,194 +650,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C40CDF-F3BA-4596-A081-51163C52FCCA}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>475</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>988</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>11.87</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
+        <v>24.5</v>
+      </c>
+      <c r="F2" s="3">
         <f>D2/B2*C2</f>
         <v>24.689599999999999</v>
       </c>
-      <c r="F2">
-        <v>24.5</v>
-      </c>
-      <c r="G2">
-        <f>F2-E2</f>
+      <c r="G2" s="3">
+        <f>E2-F2</f>
         <v>-0.18959999999999866</v>
       </c>
+      <c r="H2" s="5">
+        <v>61.6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>481</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>798</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>11.87</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="F3" s="4">
         <f>D3/B3*C3</f>
         <v>19.692848232848231</v>
       </c>
-      <c r="F3">
-        <v>21.6</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">F3-E3</f>
+      <c r="G3" s="4">
+        <f>E3-F3</f>
         <v>1.9071517671517704</v>
       </c>
+      <c r="H3" s="4">
+        <v>29.8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>478</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>571</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>11.87</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E3:E7" si="1">D4/B4*C4</f>
+      <c r="E4" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="F4" s="3">
+        <f>D4/B4*C4</f>
         <v>14.179435146443515</v>
       </c>
-      <c r="F4">
-        <v>15.1</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
+      <c r="G4" s="3">
+        <f>E4-F4</f>
         <v>0.92056485355648476</v>
       </c>
+      <c r="H4" s="3">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>475</v>
+      </c>
+      <c r="C5" s="4">
+        <v>878</v>
+      </c>
+      <c r="D5" s="4">
+        <v>11.87</v>
+      </c>
+      <c r="E5" s="4">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4">
+        <f>D5/B5*C5</f>
+        <v>21.940757894736841</v>
+      </c>
+      <c r="G5" s="4">
+        <f>E5-F5</f>
+        <v>5.9242105263159317E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>478</v>
+      </c>
+      <c r="C6" s="3">
+        <v>913</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11.87</v>
+      </c>
+      <c r="E6" s="3">
+        <v>21.7</v>
+      </c>
+      <c r="F6" s="3">
+        <f>D6/B6*C6</f>
+        <v>22.672196652719666</v>
+      </c>
+      <c r="G6" s="3">
+        <f>E6-F6</f>
+        <v>-0.97219665271966704</v>
+      </c>
+      <c r="H6" s="6">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>475</v>
-      </c>
-      <c r="C5">
-        <v>878</v>
-      </c>
-      <c r="D5">
+      <c r="B7" s="4">
+        <v>478</v>
+      </c>
+      <c r="C7" s="4">
+        <v>799</v>
+      </c>
+      <c r="D7" s="4">
         <v>11.87</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>21.940757894736841</v>
-      </c>
-      <c r="F5">
-        <v>22</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>5.9242105263159317E-2</v>
+      <c r="E7" s="4">
+        <v>21.1</v>
+      </c>
+      <c r="F7" s="4">
+        <f>D7/B7*C7</f>
+        <v>19.841276150627614</v>
+      </c>
+      <c r="G7" s="4">
+        <f>E7-F7</f>
+        <v>1.2587238493723873</v>
+      </c>
+      <c r="H7" s="4">
+        <v>64.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>478</v>
-      </c>
-      <c r="C6">
-        <v>913</v>
-      </c>
-      <c r="D6">
-        <v>11.87</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>22.672196652719666</v>
-      </c>
-      <c r="F6">
-        <v>21.7</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>-0.97219665271966704</v>
-      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>478</v>
-      </c>
-      <c r="C7">
-        <v>799</v>
-      </c>
-      <c r="D7">
-        <v>11.87</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>19.841276150627614</v>
-      </c>
-      <c r="F7">
-        <v>21.1</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1.2587238493723873</v>
-      </c>
+    <row r="13" spans="1:21" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="Q13:U13"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="Q12:U12"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>